<commit_message>
Inclusion perfil y ejemplos Claim
Inclusion perfil y ejemplos Claim
</commit_message>
<xml_diff>
--- a/fhir/indisa/StructureDefinition-ProfileServiceRequestKlinic.xlsx
+++ b/fhir/indisa/StructureDefinition-ProfileServiceRequestKlinic.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$200</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AN$206</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7199" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7414" uniqueCount="689">
   <si>
     <t>Path</t>
   </si>
@@ -1907,6 +1907,24 @@
   </si>
   <si>
     <t>.outboundRelationship[typeCode=PERT].target</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.id</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.extension</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.reference</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.type</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.identifier</t>
+  </si>
+  <si>
+    <t>ServiceRequest.supportingInfo.display</t>
   </si>
   <si>
     <t>ServiceRequest.specimen</t>
@@ -2276,7 +2294,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN200"/>
+  <dimension ref="A1:AN206"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -21952,7 +21970,7 @@
         <v>42</v>
       </c>
       <c r="F173" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G173" t="s" s="2">
         <v>44</v>
@@ -22075,20 +22093,18 @@
         <v>44</v>
       </c>
       <c r="I174" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J174" t="s" s="2">
-        <v>613</v>
+        <v>54</v>
       </c>
       <c r="K174" t="s" s="2">
-        <v>614</v>
+        <v>123</v>
       </c>
       <c r="L174" t="s" s="2">
-        <v>615</v>
-      </c>
-      <c r="M174" t="s" s="2">
-        <v>616</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="M174" s="2"/>
       <c r="N174" s="2"/>
       <c r="O174" t="s" s="2">
         <v>44</v>
@@ -22137,28 +22153,28 @@
         <v>44</v>
       </c>
       <c r="AE174" t="s" s="2">
-        <v>612</v>
+        <v>125</v>
       </c>
       <c r="AF174" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG174" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH174" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI174" t="s" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="AJ174" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK174" t="s" s="2">
-        <v>617</v>
+        <v>44</v>
       </c>
       <c r="AL174" t="s" s="2">
-        <v>618</v>
+        <v>126</v>
       </c>
       <c r="AM174" t="s" s="2">
         <v>44</v>
@@ -22169,18 +22185,18 @@
     </row>
     <row r="175" hidden="true">
       <c r="A175" t="s" s="2">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" t="s" s="2">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D175" s="2"/>
       <c r="E175" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F175" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G175" t="s" s="2">
         <v>44</v>
@@ -22192,15 +22208,17 @@
         <v>44</v>
       </c>
       <c r="J175" t="s" s="2">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="K175" t="s" s="2">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="L175" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="M175" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="M175" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="N175" s="2"/>
       <c r="O175" t="s" s="2">
         <v>44</v>
@@ -22237,31 +22255,31 @@
         <v>44</v>
       </c>
       <c r="AA175" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB175" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC175" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD175" t="s" s="2">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="AE175" t="s" s="2">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="AF175" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG175" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH175" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI175" t="s" s="2">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="AJ175" t="s" s="2">
         <v>44</v>
@@ -22281,18 +22299,18 @@
     </row>
     <row r="176" hidden="true">
       <c r="A176" t="s" s="2">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" t="s" s="2">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D176" s="2"/>
       <c r="E176" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F176" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G176" t="s" s="2">
         <v>44</v>
@@ -22301,19 +22319,19 @@
         <v>44</v>
       </c>
       <c r="I176" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J176" t="s" s="2">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="K176" t="s" s="2">
-        <v>99</v>
+        <v>215</v>
       </c>
       <c r="L176" t="s" s="2">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="M176" t="s" s="2">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="N176" s="2"/>
       <c r="O176" t="s" s="2">
@@ -22351,31 +22369,31 @@
         <v>44</v>
       </c>
       <c r="AA176" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB176" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC176" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD176" t="s" s="2">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="AE176" t="s" s="2">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="AF176" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG176" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH176" t="s" s="2">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="AI176" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ176" t="s" s="2">
         <v>44</v>
@@ -22384,7 +22402,7 @@
         <v>44</v>
       </c>
       <c r="AL176" t="s" s="2">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="AM176" t="s" s="2">
         <v>44</v>
@@ -22395,7 +22413,7 @@
     </row>
     <row r="177" hidden="true">
       <c r="A177" t="s" s="2">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" t="s" s="2">
@@ -22406,7 +22424,7 @@
         <v>42</v>
       </c>
       <c r="F177" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G177" t="s" s="2">
         <v>44</v>
@@ -22418,16 +22436,16 @@
         <v>53</v>
       </c>
       <c r="J177" t="s" s="2">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="K177" t="s" s="2">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="L177" t="s" s="2">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="M177" t="s" s="2">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="N177" s="2"/>
       <c r="O177" t="s" s="2">
@@ -22453,13 +22471,13 @@
         <v>44</v>
       </c>
       <c r="W177" t="s" s="2">
-        <v>44</v>
+        <v>149</v>
       </c>
       <c r="X177" t="s" s="2">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="Y177" t="s" s="2">
-        <v>44</v>
+        <v>225</v>
       </c>
       <c r="Z177" t="s" s="2">
         <v>44</v>
@@ -22477,7 +22495,7 @@
         <v>44</v>
       </c>
       <c r="AE177" t="s" s="2">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="AF177" t="s" s="2">
         <v>42</v>
@@ -22486,7 +22504,7 @@
         <v>52</v>
       </c>
       <c r="AH177" t="s" s="2">
-        <v>219</v>
+        <v>44</v>
       </c>
       <c r="AI177" t="s" s="2">
         <v>64</v>
@@ -22509,7 +22527,7 @@
     </row>
     <row r="178" hidden="true">
       <c r="A178" t="s" s="2">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B178" s="2"/>
       <c r="C178" t="s" s="2">
@@ -22532,16 +22550,16 @@
         <v>53</v>
       </c>
       <c r="J178" t="s" s="2">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="K178" t="s" s="2">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="L178" t="s" s="2">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="M178" t="s" s="2">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="N178" s="2"/>
       <c r="O178" t="s" s="2">
@@ -22567,13 +22585,13 @@
         <v>44</v>
       </c>
       <c r="W178" t="s" s="2">
-        <v>149</v>
+        <v>44</v>
       </c>
       <c r="X178" t="s" s="2">
-        <v>224</v>
+        <v>44</v>
       </c>
       <c r="Y178" t="s" s="2">
-        <v>225</v>
+        <v>44</v>
       </c>
       <c r="Z178" t="s" s="2">
         <v>44</v>
@@ -22591,7 +22609,7 @@
         <v>44</v>
       </c>
       <c r="AE178" t="s" s="2">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="AF178" t="s" s="2">
         <v>42</v>
@@ -22612,7 +22630,7 @@
         <v>44</v>
       </c>
       <c r="AL178" t="s" s="2">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="AM178" t="s" s="2">
         <v>44</v>
@@ -22623,7 +22641,7 @@
     </row>
     <row r="179" hidden="true">
       <c r="A179" t="s" s="2">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B179" s="2"/>
       <c r="C179" t="s" s="2">
@@ -22646,16 +22664,16 @@
         <v>53</v>
       </c>
       <c r="J179" t="s" s="2">
-        <v>110</v>
+        <v>54</v>
       </c>
       <c r="K179" t="s" s="2">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="L179" t="s" s="2">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="M179" t="s" s="2">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="N179" s="2"/>
       <c r="O179" t="s" s="2">
@@ -22705,7 +22723,7 @@
         <v>44</v>
       </c>
       <c r="AE179" t="s" s="2">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="AF179" t="s" s="2">
         <v>42</v>
@@ -22726,7 +22744,7 @@
         <v>44</v>
       </c>
       <c r="AL179" t="s" s="2">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="AM179" t="s" s="2">
         <v>44</v>
@@ -22737,7 +22755,7 @@
     </row>
     <row r="180" hidden="true">
       <c r="A180" t="s" s="2">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="B180" s="2"/>
       <c r="C180" t="s" s="2">
@@ -22748,7 +22766,7 @@
         <v>42</v>
       </c>
       <c r="F180" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G180" t="s" s="2">
         <v>44</v>
@@ -22760,16 +22778,16 @@
         <v>53</v>
       </c>
       <c r="J180" t="s" s="2">
-        <v>54</v>
+        <v>619</v>
       </c>
       <c r="K180" t="s" s="2">
-        <v>233</v>
+        <v>620</v>
       </c>
       <c r="L180" t="s" s="2">
-        <v>234</v>
+        <v>621</v>
       </c>
       <c r="M180" t="s" s="2">
-        <v>235</v>
+        <v>622</v>
       </c>
       <c r="N180" s="2"/>
       <c r="O180" t="s" s="2">
@@ -22819,13 +22837,13 @@
         <v>44</v>
       </c>
       <c r="AE180" t="s" s="2">
-        <v>236</v>
+        <v>618</v>
       </c>
       <c r="AF180" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG180" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH180" t="s" s="2">
         <v>44</v>
@@ -22837,10 +22855,10 @@
         <v>44</v>
       </c>
       <c r="AK180" t="s" s="2">
-        <v>44</v>
+        <v>623</v>
       </c>
       <c r="AL180" t="s" s="2">
-        <v>95</v>
+        <v>624</v>
       </c>
       <c r="AM180" t="s" s="2">
         <v>44</v>
@@ -22855,14 +22873,14 @@
       </c>
       <c r="B181" s="2"/>
       <c r="C181" t="s" s="2">
-        <v>626</v>
+        <v>44</v>
       </c>
       <c r="D181" s="2"/>
       <c r="E181" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F181" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G181" t="s" s="2">
         <v>44</v>
@@ -22871,23 +22889,19 @@
         <v>44</v>
       </c>
       <c r="I181" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J181" t="s" s="2">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="K181" t="s" s="2">
-        <v>627</v>
+        <v>123</v>
       </c>
       <c r="L181" t="s" s="2">
-        <v>628</v>
-      </c>
-      <c r="M181" t="s" s="2">
-        <v>629</v>
-      </c>
-      <c r="N181" t="s" s="2">
-        <v>630</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="M181" s="2"/>
+      <c r="N181" s="2"/>
       <c r="O181" t="s" s="2">
         <v>44</v>
       </c>
@@ -22911,13 +22925,13 @@
         <v>44</v>
       </c>
       <c r="W181" t="s" s="2">
-        <v>293</v>
+        <v>44</v>
       </c>
       <c r="X181" t="s" s="2">
-        <v>631</v>
+        <v>44</v>
       </c>
       <c r="Y181" t="s" s="2">
-        <v>632</v>
+        <v>44</v>
       </c>
       <c r="Z181" t="s" s="2">
         <v>44</v>
@@ -22935,50 +22949,50 @@
         <v>44</v>
       </c>
       <c r="AE181" t="s" s="2">
-        <v>625</v>
+        <v>125</v>
       </c>
       <c r="AF181" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG181" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH181" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI181" t="s" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="AJ181" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK181" t="s" s="2">
-        <v>617</v>
+        <v>44</v>
       </c>
       <c r="AL181" t="s" s="2">
-        <v>633</v>
+        <v>126</v>
       </c>
       <c r="AM181" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN181" t="s" s="2">
-        <v>634</v>
+        <v>44</v>
       </c>
     </row>
     <row r="182" hidden="true">
       <c r="A182" t="s" s="2">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="B182" s="2"/>
       <c r="C182" t="s" s="2">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D182" s="2"/>
       <c r="E182" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F182" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G182" t="s" s="2">
         <v>44</v>
@@ -22990,15 +23004,17 @@
         <v>44</v>
       </c>
       <c r="J182" t="s" s="2">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="K182" t="s" s="2">
-        <v>123</v>
+        <v>99</v>
       </c>
       <c r="L182" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="M182" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="M182" t="s" s="2">
+        <v>101</v>
+      </c>
       <c r="N182" s="2"/>
       <c r="O182" t="s" s="2">
         <v>44</v>
@@ -23035,31 +23051,31 @@
         <v>44</v>
       </c>
       <c r="AA182" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB182" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC182" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD182" t="s" s="2">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="AE182" t="s" s="2">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="AF182" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG182" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH182" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI182" t="s" s="2">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="AJ182" t="s" s="2">
         <v>44</v>
@@ -23079,18 +23095,18 @@
     </row>
     <row r="183" hidden="true">
       <c r="A183" t="s" s="2">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="B183" s="2"/>
       <c r="C183" t="s" s="2">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D183" s="2"/>
       <c r="E183" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F183" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G183" t="s" s="2">
         <v>44</v>
@@ -23099,19 +23115,19 @@
         <v>44</v>
       </c>
       <c r="I183" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J183" t="s" s="2">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="K183" t="s" s="2">
-        <v>99</v>
+        <v>215</v>
       </c>
       <c r="L183" t="s" s="2">
-        <v>128</v>
+        <v>216</v>
       </c>
       <c r="M183" t="s" s="2">
-        <v>101</v>
+        <v>217</v>
       </c>
       <c r="N183" s="2"/>
       <c r="O183" t="s" s="2">
@@ -23149,31 +23165,31 @@
         <v>44</v>
       </c>
       <c r="AA183" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB183" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC183" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD183" t="s" s="2">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="AE183" t="s" s="2">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="AF183" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG183" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH183" t="s" s="2">
-        <v>44</v>
+        <v>219</v>
       </c>
       <c r="AI183" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ183" t="s" s="2">
         <v>44</v>
@@ -23182,7 +23198,7 @@
         <v>44</v>
       </c>
       <c r="AL183" t="s" s="2">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="AM183" t="s" s="2">
         <v>44</v>
@@ -23193,7 +23209,7 @@
     </row>
     <row r="184" hidden="true">
       <c r="A184" t="s" s="2">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="B184" s="2"/>
       <c r="C184" t="s" s="2">
@@ -23204,7 +23220,7 @@
         <v>42</v>
       </c>
       <c r="F184" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G184" t="s" s="2">
         <v>44</v>
@@ -23216,20 +23232,18 @@
         <v>53</v>
       </c>
       <c r="J184" t="s" s="2">
-        <v>301</v>
+        <v>66</v>
       </c>
       <c r="K184" t="s" s="2">
-        <v>302</v>
+        <v>221</v>
       </c>
       <c r="L184" t="s" s="2">
-        <v>303</v>
+        <v>222</v>
       </c>
       <c r="M184" t="s" s="2">
-        <v>304</v>
-      </c>
-      <c r="N184" t="s" s="2">
-        <v>305</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="N184" s="2"/>
       <c r="O184" t="s" s="2">
         <v>44</v>
       </c>
@@ -23253,13 +23267,13 @@
         <v>44</v>
       </c>
       <c r="W184" t="s" s="2">
-        <v>44</v>
+        <v>149</v>
       </c>
       <c r="X184" t="s" s="2">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="Y184" t="s" s="2">
-        <v>44</v>
+        <v>225</v>
       </c>
       <c r="Z184" t="s" s="2">
         <v>44</v>
@@ -23277,13 +23291,13 @@
         <v>44</v>
       </c>
       <c r="AE184" t="s" s="2">
-        <v>306</v>
+        <v>226</v>
       </c>
       <c r="AF184" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG184" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH184" t="s" s="2">
         <v>44</v>
@@ -23295,10 +23309,10 @@
         <v>44</v>
       </c>
       <c r="AK184" t="s" s="2">
-        <v>307</v>
+        <v>44</v>
       </c>
       <c r="AL184" t="s" s="2">
-        <v>308</v>
+        <v>95</v>
       </c>
       <c r="AM184" t="s" s="2">
         <v>44</v>
@@ -23309,7 +23323,7 @@
     </row>
     <row r="185" hidden="true">
       <c r="A185" t="s" s="2">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="B185" s="2"/>
       <c r="C185" t="s" s="2">
@@ -23329,18 +23343,20 @@
         <v>44</v>
       </c>
       <c r="I185" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J185" t="s" s="2">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="K185" t="s" s="2">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="L185" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="M185" s="2"/>
+        <v>229</v>
+      </c>
+      <c r="M185" t="s" s="2">
+        <v>230</v>
+      </c>
       <c r="N185" s="2"/>
       <c r="O185" t="s" s="2">
         <v>44</v>
@@ -23389,7 +23405,7 @@
         <v>44</v>
       </c>
       <c r="AE185" t="s" s="2">
-        <v>125</v>
+        <v>231</v>
       </c>
       <c r="AF185" t="s" s="2">
         <v>42</v>
@@ -23401,7 +23417,7 @@
         <v>44</v>
       </c>
       <c r="AI185" t="s" s="2">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="AJ185" t="s" s="2">
         <v>44</v>
@@ -23410,7 +23426,7 @@
         <v>44</v>
       </c>
       <c r="AL185" t="s" s="2">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="AM185" t="s" s="2">
         <v>44</v>
@@ -23421,18 +23437,18 @@
     </row>
     <row r="186" hidden="true">
       <c r="A186" t="s" s="2">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="B186" s="2"/>
       <c r="C186" t="s" s="2">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D186" s="2"/>
       <c r="E186" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F186" t="s" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G186" t="s" s="2">
         <v>44</v>
@@ -23441,19 +23457,19 @@
         <v>44</v>
       </c>
       <c r="I186" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J186" t="s" s="2">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="K186" t="s" s="2">
-        <v>99</v>
+        <v>233</v>
       </c>
       <c r="L186" t="s" s="2">
-        <v>128</v>
+        <v>234</v>
       </c>
       <c r="M186" t="s" s="2">
-        <v>101</v>
+        <v>235</v>
       </c>
       <c r="N186" s="2"/>
       <c r="O186" t="s" s="2">
@@ -23491,31 +23507,31 @@
         <v>44</v>
       </c>
       <c r="AA186" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB186" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC186" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD186" t="s" s="2">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="AE186" t="s" s="2">
-        <v>131</v>
+        <v>236</v>
       </c>
       <c r="AF186" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG186" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH186" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI186" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ186" t="s" s="2">
         <v>44</v>
@@ -23524,7 +23540,7 @@
         <v>44</v>
       </c>
       <c r="AL186" t="s" s="2">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="AM186" t="s" s="2">
         <v>44</v>
@@ -23535,18 +23551,18 @@
     </row>
     <row r="187" hidden="true">
       <c r="A187" t="s" s="2">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="B187" s="2"/>
       <c r="C187" t="s" s="2">
-        <v>44</v>
+        <v>632</v>
       </c>
       <c r="D187" s="2"/>
       <c r="E187" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F187" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G187" t="s" s="2">
         <v>44</v>
@@ -23558,26 +23574,26 @@
         <v>53</v>
       </c>
       <c r="J187" t="s" s="2">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="K187" t="s" s="2">
-        <v>312</v>
+        <v>633</v>
       </c>
       <c r="L187" t="s" s="2">
-        <v>313</v>
+        <v>634</v>
       </c>
       <c r="M187" t="s" s="2">
-        <v>314</v>
+        <v>635</v>
       </c>
       <c r="N187" t="s" s="2">
-        <v>315</v>
+        <v>636</v>
       </c>
       <c r="O187" t="s" s="2">
         <v>44</v>
       </c>
       <c r="P187" s="2"/>
       <c r="Q187" t="s" s="2">
-        <v>316</v>
+        <v>44</v>
       </c>
       <c r="R187" t="s" s="2">
         <v>44</v>
@@ -23595,13 +23611,13 @@
         <v>44</v>
       </c>
       <c r="W187" t="s" s="2">
-        <v>44</v>
+        <v>293</v>
       </c>
       <c r="X187" t="s" s="2">
-        <v>44</v>
+        <v>637</v>
       </c>
       <c r="Y187" t="s" s="2">
-        <v>44</v>
+        <v>638</v>
       </c>
       <c r="Z187" t="s" s="2">
         <v>44</v>
@@ -23619,13 +23635,13 @@
         <v>44</v>
       </c>
       <c r="AE187" t="s" s="2">
-        <v>317</v>
+        <v>631</v>
       </c>
       <c r="AF187" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG187" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH187" t="s" s="2">
         <v>44</v>
@@ -23637,16 +23653,16 @@
         <v>44</v>
       </c>
       <c r="AK187" t="s" s="2">
-        <v>318</v>
+        <v>623</v>
       </c>
       <c r="AL187" t="s" s="2">
-        <v>319</v>
+        <v>639</v>
       </c>
       <c r="AM187" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN187" t="s" s="2">
-        <v>44</v>
+        <v>640</v>
       </c>
     </row>
     <row r="188" hidden="true">
@@ -23671,20 +23687,18 @@
         <v>44</v>
       </c>
       <c r="I188" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J188" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K188" t="s" s="2">
-        <v>321</v>
+        <v>123</v>
       </c>
       <c r="L188" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="M188" t="s" s="2">
-        <v>323</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="M188" s="2"/>
       <c r="N188" s="2"/>
       <c r="O188" t="s" s="2">
         <v>44</v>
@@ -23733,7 +23747,7 @@
         <v>44</v>
       </c>
       <c r="AE188" t="s" s="2">
-        <v>324</v>
+        <v>125</v>
       </c>
       <c r="AF188" t="s" s="2">
         <v>42</v>
@@ -23745,16 +23759,16 @@
         <v>44</v>
       </c>
       <c r="AI188" t="s" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="AJ188" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK188" t="s" s="2">
-        <v>325</v>
+        <v>44</v>
       </c>
       <c r="AL188" t="s" s="2">
-        <v>326</v>
+        <v>126</v>
       </c>
       <c r="AM188" t="s" s="2">
         <v>44</v>
@@ -23769,14 +23783,14 @@
       </c>
       <c r="B189" s="2"/>
       <c r="C189" t="s" s="2">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D189" s="2"/>
       <c r="E189" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F189" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G189" t="s" s="2">
         <v>44</v>
@@ -23785,21 +23799,21 @@
         <v>44</v>
       </c>
       <c r="I189" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J189" t="s" s="2">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="K189" t="s" s="2">
-        <v>328</v>
+        <v>99</v>
       </c>
       <c r="L189" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="M189" s="2"/>
-      <c r="N189" t="s" s="2">
-        <v>330</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="M189" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="N189" s="2"/>
       <c r="O189" t="s" s="2">
         <v>44</v>
       </c>
@@ -23835,40 +23849,40 @@
         <v>44</v>
       </c>
       <c r="AA189" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB189" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC189" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD189" t="s" s="2">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="AE189" t="s" s="2">
-        <v>331</v>
+        <v>131</v>
       </c>
       <c r="AF189" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG189" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH189" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI189" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ189" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK189" t="s" s="2">
-        <v>332</v>
+        <v>44</v>
       </c>
       <c r="AL189" t="s" s="2">
-        <v>333</v>
+        <v>126</v>
       </c>
       <c r="AM189" t="s" s="2">
         <v>44</v>
@@ -23887,10 +23901,10 @@
       </c>
       <c r="D190" s="2"/>
       <c r="E190" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F190" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G190" t="s" s="2">
         <v>44</v>
@@ -23902,17 +23916,19 @@
         <v>53</v>
       </c>
       <c r="J190" t="s" s="2">
-        <v>54</v>
+        <v>301</v>
       </c>
       <c r="K190" t="s" s="2">
-        <v>335</v>
+        <v>302</v>
       </c>
       <c r="L190" t="s" s="2">
-        <v>336</v>
-      </c>
-      <c r="M190" s="2"/>
+        <v>303</v>
+      </c>
+      <c r="M190" t="s" s="2">
+        <v>304</v>
+      </c>
       <c r="N190" t="s" s="2">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="O190" t="s" s="2">
         <v>44</v>
@@ -23961,13 +23977,13 @@
         <v>44</v>
       </c>
       <c r="AE190" t="s" s="2">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="AF190" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG190" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH190" t="s" s="2">
         <v>44</v>
@@ -23979,10 +23995,10 @@
         <v>44</v>
       </c>
       <c r="AK190" t="s" s="2">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="AL190" t="s" s="2">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="AM190" t="s" s="2">
         <v>44</v>
@@ -24013,23 +24029,19 @@
         <v>44</v>
       </c>
       <c r="I191" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J191" t="s" s="2">
-        <v>342</v>
+        <v>54</v>
       </c>
       <c r="K191" t="s" s="2">
-        <v>343</v>
+        <v>123</v>
       </c>
       <c r="L191" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="M191" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="N191" t="s" s="2">
-        <v>346</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="M191" s="2"/>
+      <c r="N191" s="2"/>
       <c r="O191" t="s" s="2">
         <v>44</v>
       </c>
@@ -24077,7 +24089,7 @@
         <v>44</v>
       </c>
       <c r="AE191" t="s" s="2">
-        <v>347</v>
+        <v>125</v>
       </c>
       <c r="AF191" t="s" s="2">
         <v>42</v>
@@ -24089,16 +24101,16 @@
         <v>44</v>
       </c>
       <c r="AI191" t="s" s="2">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="AJ191" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK191" t="s" s="2">
-        <v>348</v>
+        <v>44</v>
       </c>
       <c r="AL191" t="s" s="2">
-        <v>349</v>
+        <v>126</v>
       </c>
       <c r="AM191" t="s" s="2">
         <v>44</v>
@@ -24113,14 +24125,14 @@
       </c>
       <c r="B192" s="2"/>
       <c r="C192" t="s" s="2">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="D192" s="2"/>
       <c r="E192" t="s" s="2">
         <v>42</v>
       </c>
       <c r="F192" t="s" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G192" t="s" s="2">
         <v>44</v>
@@ -24129,23 +24141,21 @@
         <v>44</v>
       </c>
       <c r="I192" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J192" t="s" s="2">
-        <v>54</v>
+        <v>98</v>
       </c>
       <c r="K192" t="s" s="2">
-        <v>351</v>
+        <v>99</v>
       </c>
       <c r="L192" t="s" s="2">
-        <v>352</v>
+        <v>128</v>
       </c>
       <c r="M192" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="N192" t="s" s="2">
-        <v>354</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="N192" s="2"/>
       <c r="O192" t="s" s="2">
         <v>44</v>
       </c>
@@ -24181,40 +24191,40 @@
         <v>44</v>
       </c>
       <c r="AA192" t="s" s="2">
-        <v>44</v>
+        <v>129</v>
       </c>
       <c r="AB192" t="s" s="2">
-        <v>44</v>
+        <v>130</v>
       </c>
       <c r="AC192" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD192" t="s" s="2">
-        <v>44</v>
+        <v>115</v>
       </c>
       <c r="AE192" t="s" s="2">
-        <v>355</v>
+        <v>131</v>
       </c>
       <c r="AF192" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG192" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH192" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI192" t="s" s="2">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="AJ192" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK192" t="s" s="2">
-        <v>356</v>
+        <v>44</v>
       </c>
       <c r="AL192" t="s" s="2">
-        <v>357</v>
+        <v>126</v>
       </c>
       <c r="AM192" t="s" s="2">
         <v>44</v>
@@ -24233,10 +24243,10 @@
       </c>
       <c r="D193" s="2"/>
       <c r="E193" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F193" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G193" t="s" s="2">
         <v>44</v>
@@ -24245,25 +24255,29 @@
         <v>44</v>
       </c>
       <c r="I193" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J193" t="s" s="2">
-        <v>647</v>
+        <v>66</v>
       </c>
       <c r="K193" t="s" s="2">
-        <v>12</v>
+        <v>312</v>
       </c>
       <c r="L193" t="s" s="2">
-        <v>648</v>
-      </c>
-      <c r="M193" s="2"/>
-      <c r="N193" s="2"/>
+        <v>313</v>
+      </c>
+      <c r="M193" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="N193" t="s" s="2">
+        <v>315</v>
+      </c>
       <c r="O193" t="s" s="2">
         <v>44</v>
       </c>
       <c r="P193" s="2"/>
       <c r="Q193" t="s" s="2">
-        <v>44</v>
+        <v>316</v>
       </c>
       <c r="R193" t="s" s="2">
         <v>44</v>
@@ -24305,13 +24319,13 @@
         <v>44</v>
       </c>
       <c r="AE193" t="s" s="2">
-        <v>646</v>
+        <v>317</v>
       </c>
       <c r="AF193" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG193" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH193" t="s" s="2">
         <v>44</v>
@@ -24320,24 +24334,24 @@
         <v>64</v>
       </c>
       <c r="AJ193" t="s" s="2">
-        <v>649</v>
+        <v>44</v>
       </c>
       <c r="AK193" t="s" s="2">
-        <v>408</v>
+        <v>318</v>
       </c>
       <c r="AL193" t="s" s="2">
-        <v>650</v>
+        <v>319</v>
       </c>
       <c r="AM193" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN193" t="s" s="2">
-        <v>651</v>
+        <v>44</v>
       </c>
     </row>
     <row r="194" hidden="true">
       <c r="A194" t="s" s="2">
-        <v>652</v>
+        <v>647</v>
       </c>
       <c r="B194" s="2"/>
       <c r="C194" t="s" s="2">
@@ -24357,18 +24371,20 @@
         <v>44</v>
       </c>
       <c r="I194" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J194" t="s" s="2">
         <v>54</v>
       </c>
       <c r="K194" t="s" s="2">
-        <v>123</v>
+        <v>321</v>
       </c>
       <c r="L194" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="M194" s="2"/>
+        <v>322</v>
+      </c>
+      <c r="M194" t="s" s="2">
+        <v>323</v>
+      </c>
       <c r="N194" s="2"/>
       <c r="O194" t="s" s="2">
         <v>44</v>
@@ -24417,7 +24433,7 @@
         <v>44</v>
       </c>
       <c r="AE194" t="s" s="2">
-        <v>125</v>
+        <v>324</v>
       </c>
       <c r="AF194" t="s" s="2">
         <v>42</v>
@@ -24429,16 +24445,16 @@
         <v>44</v>
       </c>
       <c r="AI194" t="s" s="2">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="AJ194" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK194" t="s" s="2">
-        <v>44</v>
+        <v>325</v>
       </c>
       <c r="AL194" t="s" s="2">
-        <v>126</v>
+        <v>326</v>
       </c>
       <c r="AM194" t="s" s="2">
         <v>44</v>
@@ -24449,18 +24465,18 @@
     </row>
     <row r="195" hidden="true">
       <c r="A195" t="s" s="2">
-        <v>653</v>
+        <v>648</v>
       </c>
       <c r="B195" s="2"/>
       <c r="C195" t="s" s="2">
-        <v>97</v>
+        <v>44</v>
       </c>
       <c r="D195" s="2"/>
       <c r="E195" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F195" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G195" t="s" s="2">
         <v>44</v>
@@ -24469,21 +24485,21 @@
         <v>44</v>
       </c>
       <c r="I195" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="J195" t="s" s="2">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="K195" t="s" s="2">
-        <v>99</v>
+        <v>328</v>
       </c>
       <c r="L195" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M195" t="s" s="2">
-        <v>101</v>
-      </c>
-      <c r="N195" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="M195" s="2"/>
+      <c r="N195" t="s" s="2">
+        <v>330</v>
+      </c>
       <c r="O195" t="s" s="2">
         <v>44</v>
       </c>
@@ -24519,40 +24535,40 @@
         <v>44</v>
       </c>
       <c r="AA195" t="s" s="2">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="AB195" t="s" s="2">
-        <v>130</v>
+        <v>44</v>
       </c>
       <c r="AC195" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AD195" t="s" s="2">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="AE195" t="s" s="2">
-        <v>131</v>
+        <v>331</v>
       </c>
       <c r="AF195" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG195" t="s" s="2">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="AH195" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AI195" t="s" s="2">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="AJ195" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AK195" t="s" s="2">
-        <v>44</v>
+        <v>332</v>
       </c>
       <c r="AL195" t="s" s="2">
-        <v>126</v>
+        <v>333</v>
       </c>
       <c r="AM195" t="s" s="2">
         <v>44</v>
@@ -24563,7 +24579,7 @@
     </row>
     <row r="196" hidden="true">
       <c r="A196" t="s" s="2">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="B196" s="2"/>
       <c r="C196" t="s" s="2">
@@ -24571,10 +24587,10 @@
       </c>
       <c r="D196" s="2"/>
       <c r="E196" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F196" t="s" s="2">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="G196" t="s" s="2">
         <v>44</v>
@@ -24586,18 +24602,18 @@
         <v>53</v>
       </c>
       <c r="J196" t="s" s="2">
-        <v>655</v>
+        <v>54</v>
       </c>
       <c r="K196" t="s" s="2">
-        <v>656</v>
+        <v>335</v>
       </c>
       <c r="L196" t="s" s="2">
-        <v>657</v>
-      </c>
-      <c r="M196" t="s" s="2">
-        <v>658</v>
-      </c>
-      <c r="N196" s="2"/>
+        <v>336</v>
+      </c>
+      <c r="M196" s="2"/>
+      <c r="N196" t="s" s="2">
+        <v>337</v>
+      </c>
       <c r="O196" t="s" s="2">
         <v>44</v>
       </c>
@@ -24645,7 +24661,7 @@
         <v>44</v>
       </c>
       <c r="AE196" t="s" s="2">
-        <v>659</v>
+        <v>338</v>
       </c>
       <c r="AF196" t="s" s="2">
         <v>42</v>
@@ -24663,10 +24679,10 @@
         <v>44</v>
       </c>
       <c r="AK196" t="s" s="2">
-        <v>95</v>
+        <v>339</v>
       </c>
       <c r="AL196" t="s" s="2">
-        <v>660</v>
+        <v>340</v>
       </c>
       <c r="AM196" t="s" s="2">
         <v>44</v>
@@ -24677,7 +24693,7 @@
     </row>
     <row r="197" hidden="true">
       <c r="A197" t="s" s="2">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="B197" s="2"/>
       <c r="C197" t="s" s="2">
@@ -24700,16 +24716,20 @@
         <v>53</v>
       </c>
       <c r="J197" t="s" s="2">
-        <v>477</v>
+        <v>342</v>
       </c>
       <c r="K197" t="s" s="2">
-        <v>662</v>
+        <v>343</v>
       </c>
       <c r="L197" t="s" s="2">
-        <v>663</v>
-      </c>
-      <c r="M197" s="2"/>
-      <c r="N197" s="2"/>
+        <v>344</v>
+      </c>
+      <c r="M197" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="N197" t="s" s="2">
+        <v>346</v>
+      </c>
       <c r="O197" t="s" s="2">
         <v>44</v>
       </c>
@@ -24757,7 +24777,7 @@
         <v>44</v>
       </c>
       <c r="AE197" t="s" s="2">
-        <v>664</v>
+        <v>347</v>
       </c>
       <c r="AF197" t="s" s="2">
         <v>42</v>
@@ -24775,10 +24795,10 @@
         <v>44</v>
       </c>
       <c r="AK197" t="s" s="2">
-        <v>95</v>
+        <v>348</v>
       </c>
       <c r="AL197" t="s" s="2">
-        <v>665</v>
+        <v>349</v>
       </c>
       <c r="AM197" t="s" s="2">
         <v>44</v>
@@ -24789,7 +24809,7 @@
     </row>
     <row r="198" hidden="true">
       <c r="A198" t="s" s="2">
-        <v>666</v>
+        <v>651</v>
       </c>
       <c r="B198" s="2"/>
       <c r="C198" t="s" s="2">
@@ -24797,10 +24817,10 @@
       </c>
       <c r="D198" s="2"/>
       <c r="E198" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F198" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G198" t="s" s="2">
         <v>44</v>
@@ -24812,16 +24832,20 @@
         <v>53</v>
       </c>
       <c r="J198" t="s" s="2">
-        <v>667</v>
+        <v>54</v>
       </c>
       <c r="K198" t="s" s="2">
-        <v>668</v>
+        <v>351</v>
       </c>
       <c r="L198" t="s" s="2">
-        <v>669</v>
-      </c>
-      <c r="M198" s="2"/>
-      <c r="N198" s="2"/>
+        <v>352</v>
+      </c>
+      <c r="M198" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="N198" t="s" s="2">
+        <v>354</v>
+      </c>
       <c r="O198" t="s" s="2">
         <v>44</v>
       </c>
@@ -24869,10 +24893,10 @@
         <v>44</v>
       </c>
       <c r="AE198" t="s" s="2">
-        <v>670</v>
+        <v>355</v>
       </c>
       <c r="AF198" t="s" s="2">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="AG198" t="s" s="2">
         <v>52</v>
@@ -24887,10 +24911,10 @@
         <v>44</v>
       </c>
       <c r="AK198" t="s" s="2">
-        <v>95</v>
+        <v>356</v>
       </c>
       <c r="AL198" t="s" s="2">
-        <v>671</v>
+        <v>357</v>
       </c>
       <c r="AM198" t="s" s="2">
         <v>44</v>
@@ -24901,7 +24925,7 @@
     </row>
     <row r="199" hidden="true">
       <c r="A199" t="s" s="2">
-        <v>672</v>
+        <v>652</v>
       </c>
       <c r="B199" s="2"/>
       <c r="C199" t="s" s="2">
@@ -24912,7 +24936,7 @@
         <v>42</v>
       </c>
       <c r="F199" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G199" t="s" s="2">
         <v>44</v>
@@ -24921,16 +24945,16 @@
         <v>44</v>
       </c>
       <c r="I199" t="s" s="2">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J199" t="s" s="2">
-        <v>54</v>
+        <v>653</v>
       </c>
       <c r="K199" t="s" s="2">
-        <v>673</v>
+        <v>12</v>
       </c>
       <c r="L199" t="s" s="2">
-        <v>674</v>
+        <v>654</v>
       </c>
       <c r="M199" s="2"/>
       <c r="N199" s="2"/>
@@ -24981,13 +25005,13 @@
         <v>44</v>
       </c>
       <c r="AE199" t="s" s="2">
-        <v>672</v>
+        <v>652</v>
       </c>
       <c r="AF199" t="s" s="2">
         <v>42</v>
       </c>
       <c r="AG199" t="s" s="2">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="AH199" t="s" s="2">
         <v>44</v>
@@ -24996,24 +25020,24 @@
         <v>64</v>
       </c>
       <c r="AJ199" t="s" s="2">
-        <v>44</v>
+        <v>655</v>
       </c>
       <c r="AK199" t="s" s="2">
         <v>408</v>
       </c>
       <c r="AL199" t="s" s="2">
-        <v>675</v>
+        <v>656</v>
       </c>
       <c r="AM199" t="s" s="2">
         <v>44</v>
       </c>
       <c r="AN199" t="s" s="2">
-        <v>44</v>
+        <v>657</v>
       </c>
     </row>
     <row r="200" hidden="true">
       <c r="A200" t="s" s="2">
-        <v>676</v>
+        <v>658</v>
       </c>
       <c r="B200" s="2"/>
       <c r="C200" t="s" s="2">
@@ -25036,17 +25060,15 @@
         <v>44</v>
       </c>
       <c r="J200" t="s" s="2">
-        <v>677</v>
+        <v>54</v>
       </c>
       <c r="K200" t="s" s="2">
-        <v>678</v>
+        <v>123</v>
       </c>
       <c r="L200" t="s" s="2">
-        <v>679</v>
-      </c>
-      <c r="M200" t="s" s="2">
-        <v>680</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="M200" s="2"/>
       <c r="N200" s="2"/>
       <c r="O200" t="s" s="2">
         <v>44</v>
@@ -25095,38 +25117,716 @@
         <v>44</v>
       </c>
       <c r="AE200" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AF200" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG200" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH200" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI200" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AJ200" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK200" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL200" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="AM200" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN200" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="201" hidden="true">
+      <c r="A201" t="s" s="2">
+        <v>659</v>
+      </c>
+      <c r="B201" s="2"/>
+      <c r="C201" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="D201" s="2"/>
+      <c r="E201" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F201" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="G201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J201" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="K201" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="L201" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="M201" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="N201" s="2"/>
+      <c r="O201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P201" s="2"/>
+      <c r="Q201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA201" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AB201" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="AC201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD201" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="AE201" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="AF201" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG201" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AH201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI201" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="AJ201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AL201" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="AM201" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN201" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="202" hidden="true">
+      <c r="A202" t="s" s="2">
+        <v>660</v>
+      </c>
+      <c r="B202" s="2"/>
+      <c r="C202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D202" s="2"/>
+      <c r="E202" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F202" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I202" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J202" t="s" s="2">
+        <v>661</v>
+      </c>
+      <c r="K202" t="s" s="2">
+        <v>662</v>
+      </c>
+      <c r="L202" t="s" s="2">
+        <v>663</v>
+      </c>
+      <c r="M202" t="s" s="2">
+        <v>664</v>
+      </c>
+      <c r="N202" s="2"/>
+      <c r="O202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P202" s="2"/>
+      <c r="Q202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE202" t="s" s="2">
+        <v>665</v>
+      </c>
+      <c r="AF202" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG202" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI202" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK202" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AL202" t="s" s="2">
+        <v>666</v>
+      </c>
+      <c r="AM202" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN202" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="203" hidden="true">
+      <c r="A203" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B203" s="2"/>
+      <c r="C203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D203" s="2"/>
+      <c r="E203" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F203" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I203" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J203" t="s" s="2">
+        <v>477</v>
+      </c>
+      <c r="K203" t="s" s="2">
+        <v>668</v>
+      </c>
+      <c r="L203" t="s" s="2">
+        <v>669</v>
+      </c>
+      <c r="M203" s="2"/>
+      <c r="N203" s="2"/>
+      <c r="O203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P203" s="2"/>
+      <c r="Q203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE203" t="s" s="2">
+        <v>670</v>
+      </c>
+      <c r="AF203" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG203" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI203" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK203" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AL203" t="s" s="2">
+        <v>671</v>
+      </c>
+      <c r="AM203" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN203" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="204" hidden="true">
+      <c r="A204" t="s" s="2">
+        <v>672</v>
+      </c>
+      <c r="B204" s="2"/>
+      <c r="C204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D204" s="2"/>
+      <c r="E204" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="F204" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I204" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J204" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="K204" t="s" s="2">
+        <v>674</v>
+      </c>
+      <c r="L204" t="s" s="2">
+        <v>675</v>
+      </c>
+      <c r="M204" s="2"/>
+      <c r="N204" s="2"/>
+      <c r="O204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P204" s="2"/>
+      <c r="Q204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE204" t="s" s="2">
         <v>676</v>
       </c>
-      <c r="AF200" t="s" s="2">
-        <v>42</v>
-      </c>
-      <c r="AG200" t="s" s="2">
+      <c r="AF204" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AG204" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI204" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK204" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AL204" t="s" s="2">
+        <v>677</v>
+      </c>
+      <c r="AM204" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN204" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="205" hidden="true">
+      <c r="A205" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="B205" s="2"/>
+      <c r="C205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D205" s="2"/>
+      <c r="E205" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="G205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I205" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="J205" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="K205" t="s" s="2">
+        <v>679</v>
+      </c>
+      <c r="L205" t="s" s="2">
+        <v>680</v>
+      </c>
+      <c r="M205" s="2"/>
+      <c r="N205" s="2"/>
+      <c r="O205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P205" s="2"/>
+      <c r="Q205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE205" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="AF205" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG205" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="AH205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI205" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="AJ205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AK205" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="AL205" t="s" s="2">
+        <v>681</v>
+      </c>
+      <c r="AM205" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN205" t="s" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="206" hidden="true">
+      <c r="A206" t="s" s="2">
+        <v>682</v>
+      </c>
+      <c r="B206" s="2"/>
+      <c r="C206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="D206" s="2"/>
+      <c r="E206" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="F206" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="G206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="H206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="I206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="J206" t="s" s="2">
+        <v>683</v>
+      </c>
+      <c r="K206" t="s" s="2">
+        <v>684</v>
+      </c>
+      <c r="L206" t="s" s="2">
+        <v>685</v>
+      </c>
+      <c r="M206" t="s" s="2">
+        <v>686</v>
+      </c>
+      <c r="N206" s="2"/>
+      <c r="O206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="P206" s="2"/>
+      <c r="Q206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="R206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="S206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="T206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="U206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="V206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="W206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="X206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Y206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="Z206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AA206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AB206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AC206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AD206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AE206" t="s" s="2">
+        <v>682</v>
+      </c>
+      <c r="AF206" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="AG206" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="AH200" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AI200" t="s" s="2">
+      <c r="AH206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AI206" t="s" s="2">
         <v>64</v>
       </c>
-      <c r="AJ200" t="s" s="2">
-        <v>681</v>
-      </c>
-      <c r="AK200" t="s" s="2">
+      <c r="AJ206" t="s" s="2">
+        <v>687</v>
+      </c>
+      <c r="AK206" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="AL200" t="s" s="2">
-        <v>682</v>
-      </c>
-      <c r="AM200" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AN200" t="s" s="2">
+      <c r="AL206" t="s" s="2">
+        <v>688</v>
+      </c>
+      <c r="AM206" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AN206" t="s" s="2">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AN200">
+  <autoFilter ref="A1:AN206">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -25136,7 +25836,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI199">
+  <conditionalFormatting sqref="A2:AI205">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>